<commit_message>
Test analysis without single colors
</commit_message>
<xml_diff>
--- a/Data/flow/Human_Clinical/Manual_gating.xlsx
+++ b/Data/flow/Human_Clinical/Manual_gating.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/_henaolab/Documents/R/Data/Smegmatis/Data/flow/Colombia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/_henaolab/Documents/R/Data/Methods/Data/flow/Human_Clinical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00E1D305-89EE-7C48-9B42-560B340598D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F81CDF2-FA15-964A-A12E-38E6653D726C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16400" yWindow="6420" windowWidth="28040" windowHeight="17440" xr2:uid="{2793936B-7C19-7542-9C1F-2C2FE54D67F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="with_SC" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="35">
   <si>
     <t>Pop1</t>
   </si>
@@ -515,7 +516,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,15 +581,15 @@
         <v>0.25641718000000002</v>
       </c>
       <c r="C4">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0.24185439821734286</v>
+        <f>100*C4/C$17</f>
+        <v>0.15761297861354928</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>1.4562781782657158E-2</v>
+        <v>9.8804201386450741E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -599,15 +600,15 @@
         <v>1.6194770000000001E-2</v>
       </c>
       <c r="C5">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>0.15761297861354928</v>
+        <f>100*C5/C$17</f>
+        <v>0.24185439821734286</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>-0.14141820861354928</v>
+        <v>-0.22565962821734287</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -656,15 +657,15 @@
         <v>9.1770359999999995E-2</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>1.0869860594037882E-2</v>
+        <f>100*C8/C$17</f>
+        <v>0</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>8.0900499405962112E-2</v>
+        <v>9.1770359999999995E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -675,15 +676,15 @@
         <v>9.4469490000000003E-2</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>100*C9/C$17</f>
+        <v>1.0869860594037882E-2</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>9.4469490000000003E-2</v>
+        <v>8.359962940596212E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -713,15 +714,15 @@
         <v>0.16464682</v>
       </c>
       <c r="C11">
-        <v>295</v>
+        <v>2517</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>0.8016522188102938</v>
+        <f>100*C11/C$17</f>
+        <v>6.8398597787983366</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>-0.63700539881029383</v>
+        <v>-6.6752129587983369</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -732,15 +733,15 @@
         <v>1.7949202399999999</v>
       </c>
       <c r="C12">
-        <v>2517</v>
+        <v>295</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>6.8398597787983366</v>
+        <f>100*C12/C$17</f>
+        <v>0.8016522188102938</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>-5.0449395387983369</v>
+        <v>0.99326802118970614</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -798,25 +799,6 @@
       <c r="E15">
         <f t="shared" si="1"/>
         <v>0.39359595613875381</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16">
-        <v>0.11876164</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="1"/>
-        <v>0.11876164</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">
@@ -830,6 +812,325 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92FD5CD7-5FA6-C24D-8CAA-FF8E77F5FC2B}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>19.93576075</v>
+      </c>
+      <c r="C2">
+        <v>6293</v>
+      </c>
+      <c r="D2">
+        <f>100*C2/C$17</f>
+        <v>17.101008179570098</v>
+      </c>
+      <c r="E2">
+        <f>B2-D2</f>
+        <v>2.8347525704299024</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>7.5710545500000004</v>
+      </c>
+      <c r="C3">
+        <v>8563</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D16" si="0">100*C3/C$17</f>
+        <v>23.269654066686595</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E16" si="1">B3-D3</f>
+        <v>-15.698599516686595</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.25641718000000002</v>
+      </c>
+      <c r="C4">
+        <v>89</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.24185439821734286</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>1.4562781782657158E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1.6194770000000001E-2</v>
+      </c>
+      <c r="C5">
+        <v>58</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.15761297861354928</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>-0.14141820861354928</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>20.29744393</v>
+      </c>
+      <c r="C6">
+        <v>4637</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>12.600885893638415</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>7.6965580363615853</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1.2712893700000001</v>
+      </c>
+      <c r="C7">
+        <v>578</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1.5706948558384739</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>-0.29940548583847382</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>9.1770359999999995E-2</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1.0869860594037882E-2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>8.0900499405962112E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>9.4469490000000003E-2</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>9.4469490000000003E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>38.683905099999997</v>
+      </c>
+      <c r="C10">
+        <v>12086</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>32.843283784885458</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>5.8406213151145394</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0.16464682</v>
+      </c>
+      <c r="C11">
+        <v>295</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0.8016522188102938</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>-0.63700539881029383</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12">
+        <v>1.7949202399999999</v>
+      </c>
+      <c r="C12">
+        <v>2517</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>6.8398597787983366</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>-5.0449395387983369</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13">
+        <v>1.349564E-2</v>
+      </c>
+      <c r="C13">
+        <v>137</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0.37229272534579744</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>-0.35879708534579746</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <v>0.75845501999999998</v>
+      </c>
+      <c r="C14">
+        <v>17</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>4.6196907524660998E-2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>0.71225811247533899</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15">
+        <v>0.46425005000000003</v>
+      </c>
+      <c r="C15">
+        <v>26</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>7.0654093861246228E-2</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>0.39359595613875381</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16">
+        <v>0.11876164</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>0.11876164</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>36799</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB2664C-EC1B-7C47-B5B0-236B8101E36E}">
   <dimension ref="A1:O23"/>
   <sheetViews>

</xml_diff>